<commit_message>
upgrade the StatisticsUnit feature
</commit_message>
<xml_diff>
--- a/AutoRegularInspection/统计单位表.xlsx
+++ b/AutoRegularInspection/统计单位表.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eamdf\source\repos\AutoRegularInspection\AutoRegularInspection\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFF3A624-DE73-4B40-B403-32A2B948C20E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5331FD8-379B-4698-819C-787BF2B583AD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="单位1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="20">
   <si>
     <t>序号</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -95,6 +95,30 @@
   </si>
   <si>
     <t>m\u00B3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>长度</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>面积</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>体积</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>物理量</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>无</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -429,15 +453,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="A5:D5"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -450,8 +472,11 @@
       <c r="D1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -464,8 +489,11 @@
       <c r="D2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -478,8 +506,11 @@
       <c r="D3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -492,8 +523,11 @@
       <c r="D4">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -505,20 +539,24 @@
       </c>
       <c r="D5">
         <v>3</v>
+      </c>
+      <c r="E5" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22358399-DEA5-4189-8531-1F6D7326B309}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -526,7 +564,7 @@
     <col min="2" max="2" width="8.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -539,8 +577,11 @@
       <c r="D1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -553,8 +594,11 @@
       <c r="D2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="E2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -567,8 +611,11 @@
       <c r="D3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -581,8 +628,11 @@
       <c r="D4">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -594,6 +644,9 @@
       </c>
       <c r="D5">
         <v>3</v>
+      </c>
+      <c r="E5" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>